<commit_message>
Insert Cost Calculation Industrial
</commit_message>
<xml_diff>
--- a/data/cost/PLA_cost_ind.xlsx
+++ b/data/cost/PLA_cost_ind.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974DBEB4-EEBA-AB4E-919C-F66D68967958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBEA1AF-E5B5-F34E-9484-993421E8D893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="500" windowWidth="21740" windowHeight="18240" activeTab="3" xr2:uid="{9E23791E-A9D1-B24D-9D6E-42C1F180DBE7}"/>
+    <workbookView xWindow="11860" yWindow="4720" windowWidth="21740" windowHeight="16280" activeTab="3" xr2:uid="{9E23791E-A9D1-B24D-9D6E-42C1F180DBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="shredding" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,16 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -94,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +116,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,17 +156,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CECAF4-10EE-7547-8F9A-E08E88E519F7}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="G1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,33 +525,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -579,37 +611,41 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3500</v>
+        <v>11260</v>
       </c>
       <c r="B3">
-        <v>5.7099999999999999E-5</v>
+        <f>0.0000571*0.016</f>
+        <v>9.1360000000000003E-7</v>
       </c>
       <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>5.7099999999999999E-5</v>
+        <v>30</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9.1360000000000003E-7</v>
       </c>
       <c r="E3">
-        <v>0.13800000000000001</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="H3">
-        <v>8.3000000000000004E-2</v>
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H3" s="5">
+        <f>0.083*0.128</f>
+        <v>1.0624000000000001E-2</v>
       </c>
       <c r="I3">
-        <v>0.05</v>
+        <f>0.05*0.128</f>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="J3">
-        <v>0.33</v>
+        <f>0.33*0.128</f>
+        <v>4.224E-2</v>
       </c>
       <c r="K3">
-        <v>75.41</v>
+        <v>21</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -649,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14329C3B-818D-974A-839B-1CDF92A21CC9}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="G1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,33 +712,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -762,37 +798,41 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>6000</v>
+        <v>100000</v>
       </c>
       <c r="B3">
-        <v>8.0000000000000004E-4</v>
+        <f>1.27*10^-6</f>
+        <v>1.2699999999999999E-6</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>8.0000000000000004E-4</v>
+        <f>1.27*10^-6</f>
+        <v>1.2699999999999999E-6</v>
       </c>
       <c r="E3">
-        <v>0.41699999999999998</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.33</v>
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H3" s="5">
+        <f>0.083*0.16</f>
+        <v>1.328E-2</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>8.3000000000000004E-2</v>
+        <f>0.33*0.16</f>
+        <v>5.2800000000000007E-2</v>
       </c>
       <c r="K3">
-        <v>75.41</v>
+        <v>21</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -832,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F903924-2D1B-F649-8D6E-329FE2160CED}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="125" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -859,33 +899,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1015,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C261B8B2-5703-4A47-9A2B-A87AD92FEE9B}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,34 +1082,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1129,26 +1169,26 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>10000</v>
+        <v>48940</v>
       </c>
       <c r="B3">
-        <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="C3" s="3">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="E3">
-        <f>0.436+2.844</f>
-        <v>3.28</v>
+        <f>0.0027*53/6000</f>
+        <v>2.385E-5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2.385E-5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>35.1</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>4.3900000000000002E-2</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="H3">
         <v>8.3000000000000004E-2</v>
@@ -1156,11 +1196,11 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="J3" s="7">
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="K3">
-        <v>75.41</v>
+        <v>21</v>
       </c>
       <c r="L3">
         <v>0</v>

</xml_diff>